<commit_message>
Cleaned code and added 1
</commit_message>
<xml_diff>
--- a/institutes.xlsx
+++ b/institutes.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="416">
   <si>
     <t>Region</t>
   </si>
@@ -38,6 +38,57 @@
     <t>Asia, East</t>
   </si>
   <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Beijing</t>
+  </si>
+  <si>
+    <t>Chinese Institute For Brain Research</t>
+  </si>
+  <si>
+    <t>http://en.cibr.ac.cn/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/China+International+Institute+of+Neuroscience/@39.8770921,116.3832055,13z/data=!4m8!1m2!2m1!1sChina+international+neuroscience!3m4!1s0x35f04d8532f9420d:0x8809df9b11eaf3e0!8m2!3d39.889762!4d116.362423</t>
+  </si>
+  <si>
+    <t>Peking</t>
+  </si>
+  <si>
+    <t>Peking University</t>
+  </si>
+  <si>
+    <t>http://nri.bjmu.edu.cn/english/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Peking+University/@39.986913,116.270855,13z/data=!4m8!1m2!2m1!1speking+neuroscience!3m4!1s0x35f0514b0d02a275:0x7bc19cd881ca04cb!8m2!3d39.986913!4d116.3058739</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
+    <t>Shanghai Institutes for Biological Sciences</t>
+  </si>
+  <si>
+    <t>http://www.ion.ac.cn/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Shanghai+Institutes+for+Biological+Sciences/@31.1622842,121.4047059,17z/data=!3m1!4b1!4m5!3m4!1s0x35b2648ea2678199:0xad8a1f12491b4bda!8m2!3d31.1622842!4d121.4068946</t>
+  </si>
+  <si>
+    <t>Wuhan</t>
+  </si>
+  <si>
+    <t>Institute for Brain Research Huazhong University of Science &amp; Technology</t>
+  </si>
+  <si>
+    <t>https://www.google.com/search?q=Institute+for+Brain+Research+HUST&amp;safe=active&amp;sxsrf=ALeKk03AoKrlF5kLSumQE-Z5N5hJQlk1JA%3A1616256779526&amp;ei=Cx9WYOSsH47rrgT3iKnwDg&amp;oq=Institute+for+Brain+Research+HUST&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBwghEAoQoAEyBwghEAoQoAE6BggAEBYQHjoICCEQFhAdEB46BQghEKABUNIfWJwnYKUsaABwAngAgAGPAogBzQeSAQUwLjMuMpgBAKABAaoBB2d3cy13aXrAAQE&amp;sclient=gws-wiz&amp;ved=0ahUKEwik3tXZob_vAhWOtYsKHXdECu4Q4dUDCA4&amp;uact=5</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Institute+for+Brain+Research+Huazhong+University+of+Science+%26+Technology/@30.4571118,113.8488827,9.81z/data=!4m5!3m4!1s0x342eae8ccf356c79:0x8111a528d9ebb80b!8m2!3d30.580727!4d114.26218</t>
+  </si>
+  <si>
     <t>Japan</t>
   </si>
   <si>
@@ -92,63 +143,24 @@
     <t>https://www.google.com/maps/place/Seoul+National+University/@37.4565095,126.9321611,14z/data=!4m8!1m2!2m1!1sNeuroscience+Research+Institute,+SNU!3m4!1s0x357c9fe8a0a1e2a5:0xa1e2eebc04f0c5e7!8m2!3d37.4565095!4d126.9500385</t>
   </si>
   <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Peking</t>
-  </si>
-  <si>
-    <t>Peking University</t>
-  </si>
-  <si>
-    <t>http://nri.bjmu.edu.cn/english/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Peking+University/@39.986913,116.270855,13z/data=!4m8!1m2!2m1!1speking+neuroscience!3m4!1s0x35f0514b0d02a275:0x7bc19cd881ca04cb!8m2!3d39.986913!4d116.3058739</t>
-  </si>
-  <si>
-    <t>Shanghai</t>
-  </si>
-  <si>
-    <t>Shanghai Institutes for Biological Sciences</t>
-  </si>
-  <si>
-    <t>http://www.ion.ac.cn/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Shanghai+Institutes+for+Biological+Sciences/@31.1622842,121.4047059,17z/data=!3m1!4b1!4m5!3m4!1s0x35b2648ea2678199:0xad8a1f12491b4bda!8m2!3d31.1622842!4d121.4068946</t>
-  </si>
-  <si>
-    <t>Beijing</t>
-  </si>
-  <si>
-    <t>Chinese Institute For Brain Research</t>
-  </si>
-  <si>
-    <t>http://en.cibr.ac.cn/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/China+International+Institute+of+Neuroscience/@39.8770921,116.3832055,13z/data=!4m8!1m2!2m1!1sChina+international+neuroscience!3m4!1s0x35f04d8532f9420d:0x8809df9b11eaf3e0!8m2!3d39.889762!4d116.362423</t>
-  </si>
-  <si>
-    <t>Wuhan</t>
-  </si>
-  <si>
-    <t>Institute for Brain Research Huazhong University of Science &amp; Technology</t>
-  </si>
-  <si>
-    <t>https://www.google.com/search?q=Institute+for+Brain+Research+HUST&amp;safe=active&amp;sxsrf=ALeKk03AoKrlF5kLSumQE-Z5N5hJQlk1JA%3A1616256779526&amp;ei=Cx9WYOSsH47rrgT3iKnwDg&amp;oq=Institute+for+Brain+Research+HUST&amp;gs_lcp=Cgdnd3Mtd2l6EAMyBwghEAoQoAEyBwghEAoQoAE6BggAEBYQHjoICCEQFhAdEB46BQghEKABUNIfWJwnYKUsaABwAngAgAGPAogBzQeSAQUwLjMuMpgBAKABAaoBB2d3cy13aXrAAQE&amp;sclient=gws-wiz&amp;ved=0ahUKEwik3tXZob_vAhWOtYsKHXdECu4Q4dUDCA4&amp;uact=5</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Institute+for+Brain+Research+Huazhong+University+of+Science+%26+Technology/@30.4571118,113.8488827,9.81z/data=!4m5!3m4!1s0x342eae8ccf356c79:0x8111a528d9ebb80b!8m2!3d30.580727!4d114.26218</t>
-  </si>
-  <si>
     <t>Asia, South</t>
   </si>
   <si>
     <t>India</t>
   </si>
   <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Indian Institute of Science</t>
+  </si>
+  <si>
+    <t>http://www.cns.iisc.ac.in/home/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Indian+Institute+of+Science/@13.0099733,77.558706,14z/data=!4m8!1m2!2m1!1sindian+institute+of+science+bangalore!3m4!1s0x3bae17d757d11bfb:0x3fc1cd64d345c13f!8m2!3d13.0218597!4d77.5671423</t>
+  </si>
+  <si>
     <t>Kolkata</t>
   </si>
   <si>
@@ -161,18 +173,6 @@
     <t>https://www.google.com/maps/place/Institute+of+Neurosciences+Kolkata/@22.5469568,88.3619186,15z/data=!4m5!3m4!1s0x0:0x2122bbd8d5525fb!8m2!3d22.5469568!4d88.3619186</t>
   </si>
   <si>
-    <t>Bangalore</t>
-  </si>
-  <si>
-    <t>Indian Institute of Science</t>
-  </si>
-  <si>
-    <t>http://www.cns.iisc.ac.in/home/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Indian+Institute+of+Science/@13.0099733,77.558706,14z/data=!4m8!1m2!2m1!1sindian+institute+of+science+bangalore!3m4!1s0x3bae17d757d11bfb:0x3fc1cd64d345c13f!8m2!3d13.0218597!4d77.5671423</t>
-  </si>
-  <si>
     <t>Europe, Central</t>
   </si>
   <si>
@@ -227,9 +227,87 @@
     <t>Europe, North</t>
   </si>
   <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Aarhus</t>
+  </si>
+  <si>
+    <t>NeuroCampus</t>
+  </si>
+  <si>
+    <t>https://neurocampus.au.dk/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/DANDRITE+-+Danish+Research+Institute+of+Translational+Neuroscience/@56.1669443,10.1932648,15z/data=!4m8!1m2!2m1!1saarhus+neuroscience!3m4!1s0x464c3fc3dfccd82d:0xbac74baeabdd3f63!8m2!3d56.167832!4d10.19449</t>
+  </si>
+  <si>
+    <t>Copenhagen</t>
+  </si>
+  <si>
+    <t>University of Copenhagen</t>
+  </si>
+  <si>
+    <t>https://in.ku.dk/research-themes/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Copenhagen+University/@55.6803836,12.568622,16.49z/data=!4m5!3m4!1s0x4652530f5eee9937:0x36dad5d8cf5f96fd!8m2!3d55.6802303!4d12.5724096</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Helsinki</t>
+  </si>
+  <si>
+    <t>University of Helsinki</t>
+  </si>
+  <si>
+    <t>https://www.helsinki.fi/en/hilife-neuroscience-center</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/University+of+Helsinki/@60.1700613,24.9399886,15.04z/data=!4m8!1m2!2m1!1shelsinki+neuroscience!3m4!1s0x46920a2a2fe9d929:0x3e38eb919fa64762!8m2!3d60.1726348!4d24.9510419</t>
+  </si>
+  <si>
     <t>Norway</t>
   </si>
   <si>
+    <t>Bergen</t>
+  </si>
+  <si>
+    <t>University of Bergen</t>
+  </si>
+  <si>
+    <t>https://www.uib.no/en/rg/neurosci</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/University+of+Bergen/@60.4081149,5.1856547,10.2z/data=!4m8!1m2!2m1!1sbergen+neuroscience!3m4!1s0x463cfeaaf308b829:0x7ad5dc29c0070c5e!8m2!3d60.3878586!4d5.3217549</t>
+  </si>
+  <si>
+    <t>Oslo</t>
+  </si>
+  <si>
+    <t>University of Oslo</t>
+  </si>
+  <si>
+    <t>https://www.med.uio.no/imb/english/research/about/priorities/neuro-science/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/University+of+Oslo/@59.940288,10.7096755,14.48z/data=!4m5!3m4!1s0x46416de68acb7953:0xdc70e34deaafd75d!8m2!3d59.9399586!4d10.7217496</t>
+  </si>
+  <si>
+    <t>Tromsø</t>
+  </si>
+  <si>
+    <t>University of Tromsø</t>
+  </si>
+  <si>
+    <t>https://en.uit.no/startsida</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/UiT+The+Arctic+University+of+Norway/@69.6798027,18.9712161,15z/data=!4m5!3m4!1s0x0:0x8e1ca840aebe3293!8m2!3d69.6798027!4d18.9712161</t>
+  </si>
+  <si>
     <t>Trondheim</t>
   </si>
   <si>
@@ -242,60 +320,21 @@
     <t>https://www.google.com/maps/place/Kavli+Institute+for+Systems+Neuroscience,+NTNU/@63.420693,10.3925233,15z/data=!4m5!3m4!1s0x0:0xf6ecd2e6763846bc!8m2!3d63.420693!4d10.3925233</t>
   </si>
   <si>
-    <t>Oslo</t>
-  </si>
-  <si>
-    <t>University of Oslo</t>
-  </si>
-  <si>
-    <t>https://www.med.uio.no/imb/english/research/about/priorities/neuro-science/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/University+of+Oslo/@59.940288,10.7096755,14.48z/data=!4m5!3m4!1s0x46416de68acb7953:0xdc70e34deaafd75d!8m2!3d59.9399586!4d10.7217496</t>
-  </si>
-  <si>
-    <t>Bergen</t>
-  </si>
-  <si>
-    <t>University of Bergen</t>
-  </si>
-  <si>
-    <t>https://www.uib.no/en/rg/neurosci</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/University+of+Bergen/@60.4081149,5.1856547,10.2z/data=!4m8!1m2!2m1!1sbergen+neuroscience!3m4!1s0x463cfeaaf308b829:0x7ad5dc29c0070c5e!8m2!3d60.3878586!4d5.3217549</t>
-  </si>
-  <si>
-    <t>Denmark</t>
-  </si>
-  <si>
-    <t>Aarhus</t>
-  </si>
-  <si>
-    <t>NeuroCampus</t>
-  </si>
-  <si>
-    <t>https://neurocampus.au.dk/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/DANDRITE+-+Danish+Research+Institute+of+Translational+Neuroscience/@56.1669443,10.1932648,15z/data=!4m8!1m2!2m1!1saarhus+neuroscience!3m4!1s0x464c3fc3dfccd82d:0xbac74baeabdd3f63!8m2!3d56.167832!4d10.19449</t>
-  </si>
-  <si>
-    <t>Copenhagen</t>
-  </si>
-  <si>
-    <t>University of Copenhagen</t>
-  </si>
-  <si>
-    <t>https://in.ku.dk/research-themes/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Copenhagen+University/@55.6803836,12.568622,16.49z/data=!4m5!3m4!1s0x4652530f5eee9937:0x36dad5d8cf5f96fd!8m2!3d55.6802303!4d12.5724096</t>
-  </si>
-  <si>
     <t>Sweden</t>
   </si>
   <si>
+    <t>Lund</t>
+  </si>
+  <si>
+    <t>Lund University</t>
+  </si>
+  <si>
+    <t>https://www.neuroscience.lu.se/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Lund+University/@55.7119513,13.2013043,17z/data=!3m1!4b1!4m5!3m4!1s0x465397cee93cef63:0x8f36836d04b3948a!8m2!3d55.7119483!4d13.203493</t>
+  </si>
+  <si>
     <t>Stockholm</t>
   </si>
   <si>
@@ -308,45 +347,6 @@
     <t>https://www.google.com/maps/place/Karolinska+University+Hospital/@59.3482931,18.0281873,17z/data=!3m1!4b1!4m5!3m4!1s0x465f9d9fb6e92823:0x2c8847e29aae5341!8m2!3d59.3482904!4d18.0303759</t>
   </si>
   <si>
-    <t>Lund</t>
-  </si>
-  <si>
-    <t>Lund University</t>
-  </si>
-  <si>
-    <t>https://www.neuroscience.lu.se/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Lund+University/@55.7119513,13.2013043,17z/data=!3m1!4b1!4m5!3m4!1s0x465397cee93cef63:0x8f36836d04b3948a!8m2!3d55.7119483!4d13.203493</t>
-  </si>
-  <si>
-    <t>Finland</t>
-  </si>
-  <si>
-    <t>Helsinki</t>
-  </si>
-  <si>
-    <t>University of Helsinki</t>
-  </si>
-  <si>
-    <t>https://www.helsinki.fi/en/hilife-neuroscience-center</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/University+of+Helsinki/@60.1700613,24.9399886,15.04z/data=!4m8!1m2!2m1!1shelsinki+neuroscience!3m4!1s0x46920a2a2fe9d929:0x3e38eb919fa64762!8m2!3d60.1726348!4d24.9510419</t>
-  </si>
-  <si>
-    <t>Tromsø</t>
-  </si>
-  <si>
-    <t>University of Tromsø</t>
-  </si>
-  <si>
-    <t>https://en.uit.no/startsida</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/UiT+The+Arctic+University+of+Norway/@69.6798027,18.9712161,15z/data=!4m5!3m4!1s0x0:0x8e1ca840aebe3293!8m2!3d69.6798027!4d18.9712161</t>
-  </si>
-  <si>
     <t>Europe, South</t>
   </si>
   <si>
@@ -365,6 +365,15 @@
     <t>https://www.google.com/maps/place/EMBL+Rome/@42.085073,12.5939962,15z/data=!4m5!3m4!1s0x0:0x6372467d81070dba!8m2!3d42.085073!4d12.5939962</t>
   </si>
   <si>
+    <t>Sapienza University of Rome</t>
+  </si>
+  <si>
+    <t>https://www.uniroma1.it/it/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Sapienza+University+of+Rome/@41.9037626,12.5144384,15z/data=!4m5!3m4!1s0x0:0xed5342b156dcfd2b!8m2!3d41.9037626!4d12.5144384</t>
+  </si>
+  <si>
     <t>Trieste</t>
   </si>
   <si>
@@ -377,6 +386,21 @@
     <t>https://www.google.com/maps/place/Sissa+(International+School+for+Advanced+Studies)/@45.6798192,13.7663059,15z/data=!4m8!1m2!2m1!1strieste+neuroscience!3m4!1s0x477b6b5347fa4dc3:0x6e94dec68212367b!8m2!3d45.6798192!4d13.7750606</t>
   </si>
   <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Lisbon</t>
+  </si>
+  <si>
+    <t>Champalimaud</t>
+  </si>
+  <si>
+    <t>http://first.fchampalimaud.org/en/the-foundation/champalimaud-centre-unknown/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Champalimaud+Foundation/@38.6932032,-9.2208869,15z/data=!4m2!3m1!1s0x0:0x93b51451a062a591?sa=X&amp;ved=2ahUKEwj0rNKW277vAhVLxIsKHecMCAIQ_BIwEnoECCMQBQ</t>
+  </si>
+  <si>
     <t>Spain</t>
   </si>
   <si>
@@ -392,19 +416,16 @@
     <t>https://www.google.com/maps/place/Instituto+de+Neurociencias/@38.3879238,-0.4362867,15z/data=!4m5!3m4!1s0x0:0x2ee8ac39090678d1!8m2!3d38.3879238!4d-0.4362867</t>
   </si>
   <si>
-    <t>Portugal</t>
-  </si>
-  <si>
-    <t>Lisbon</t>
-  </si>
-  <si>
-    <t>Champalimaud</t>
-  </si>
-  <si>
-    <t>http://first.fchampalimaud.org/en/the-foundation/champalimaud-centre-unknown/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Champalimaud+Foundation/@38.6932032,-9.2208869,15z/data=!4m2!3m1!1s0x0:0x93b51451a062a591?sa=X&amp;ved=2ahUKEwj0rNKW277vAhVLxIsKHecMCAIQ_BIwEnoECCMQBQ</t>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t>Institute of Neurosciences of the Universitat de Barcelona</t>
+  </si>
+  <si>
+    <t>http://www.neurociencies.ub.edu/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Institut+de+Neuroci%C3%A8ncies+UB/@41.3666385,2.0074672,10.71z/data=!4m8!1m2!2m1!1sbarcelona+neuroscience!3m4!1s0x12a497e1095cf723:0xd374fec544f41eb5!8m2!3d41.4379815!4d2.1423265</t>
   </si>
   <si>
     <t>Madrid</t>
@@ -419,18 +440,6 @@
     <t>https://www.google.com/maps/place/Cajal+Institute/@40.4482422,-3.6802321,15z/data=!4m2!3m1!1s0x0:0xb35f154ebd25a71?sa=X&amp;ved=2ahUKEwjs8sbG9b_vAhUMxosKHfZKDZUQ_BIwEnoECCAQBQ</t>
   </si>
   <si>
-    <t>Barcelona</t>
-  </si>
-  <si>
-    <t>Institute of Neurosciences of the Universitat de Barcelona</t>
-  </si>
-  <si>
-    <t>http://www.neurociencies.ub.edu/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Institut+de+Neuroci%C3%A8ncies+UB/@41.3666385,2.0074672,10.71z/data=!4m8!1m2!2m1!1sbarcelona+neuroscience!3m4!1s0x12a497e1095cf723:0xd374fec544f41eb5!8m2!3d41.4379815!4d2.1423265</t>
-  </si>
-  <si>
     <t>Seville</t>
   </si>
   <si>
@@ -443,18 +452,363 @@
     <t>https://www.google.com/maps/place/Edificio+de+Laboratorios/@37.3628046,-5.9817699,17z/data=!3m1!4b1!4m5!3m4!1s0xd126e811e8c805f:0xe2a613f9a9b3975!8m2!3d37.3628004!4d-5.9795812</t>
   </si>
   <si>
-    <t>Sapienza University of Rome</t>
-  </si>
-  <si>
-    <t>https://www.uniroma1.it/it/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Sapienza+University+of+Rome/@41.9037626,12.5144384,15z/data=!4m5!3m4!1s0x0:0xed5342b156dcfd2b!8m2!3d41.9037626!4d12.5144384</t>
-  </si>
-  <si>
     <t>Europe, West</t>
   </si>
   <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Brussels</t>
+  </si>
+  <si>
+    <t>ULB Neuroscience Institute</t>
+  </si>
+  <si>
+    <t>https://uni.ulb.ac.be/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Universit%C3%A9+Libre+de+Bruxelles/@50.8132102,4.3800335,17z/data=!3m1!4b1!4m5!3m4!1s0x47c3c4485d19ce43:0xe8eb9253c07c6691!8m2!3d50.8132068!4d4.3822222</t>
+  </si>
+  <si>
+    <t>Leuven</t>
+  </si>
+  <si>
+    <t>KU Leuven</t>
+  </si>
+  <si>
+    <t>https://www.kuleuven.be/kuleuven/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Katholieke+Universiteit+Leuven/@50.8779545,4.7002953,15z/data=!4m5!3m4!1s0x0:0x2cf72ac3db15442d!8m2!3d50.8779545!4d4.7002953</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Bristol</t>
+  </si>
+  <si>
+    <t>University of Bristol</t>
+  </si>
+  <si>
+    <t>http://www.bristol.ac.uk/neuroscience/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/University+of+Bristol/@51.4584074,-2.6037595,18.18z/data=!4m5!3m4!1s0x48718ddbdfd292fb:0x2f0b60f89b4b6d56!8m2!3d51.4584172!4d-2.6029792</t>
+  </si>
+  <si>
+    <t>Cambridge</t>
+  </si>
+  <si>
+    <t>University of Cambridge</t>
+  </si>
+  <si>
+    <t>http://www.cam.ac.uk/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/University+of+Cambridge/@52.2042666,0.1149085,15z/data=!4m5!3m4!1s0x0:0x21ca80abf36db5bb!8m2!3d52.2042666!4d0.1149085</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Cardiff University</t>
+  </si>
+  <si>
+    <t>https://www.cardiff.ac.uk/neuroscience-mental-health/research</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Cardiff+University/@51.4814204,-3.184425,14.41z/data=!4m8!1m2!2m1!1scardiff+neuroscience!3m4!1s0x0:0xe06dc7099e7122ca!8m2!3d51.4866276!4d-3.1788683</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>King's College</t>
+  </si>
+  <si>
+    <t>https://www.kcl.ac.uk/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/King's+College+London/@51.5114864,-0.115997,15z/data=!4m5!3m4!1s0x0:0xb0643efb7ed0928d!8m2!3d51.5114864!4d-0.115997</t>
+  </si>
+  <si>
+    <t>UCL</t>
+  </si>
+  <si>
+    <t>https://www.ucl.ac.uk/research/domains/neuroscience</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/UCL+Institute+of+Cognitive+Neuroscience/@51.5221999,-0.1254988,17z/data=!3m1!4b1!4m5!3m4!1s0x48761b36ce873581:0xa29303ad768432d5!8m2!3d51.5221999!4d-0.1233101</t>
+  </si>
+  <si>
+    <t>Oxford</t>
+  </si>
+  <si>
+    <t>University of Oxford</t>
+  </si>
+  <si>
+    <t>https://www.neuroscience.ox.ac.uk/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/University+of+Oxford/@51.710979,-1.3093672,12z/data=!4m8!1m2!2m1!1soxford+neuroscience!3m4!1s0x4876c6a9ef8c485b:0xd2ff1883a001afed!8m2!3d51.7548164!4d-1.2543668</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Bordeaux</t>
+  </si>
+  <si>
+    <t>Bordeaux Neurocampus</t>
+  </si>
+  <si>
+    <t>https://www.bordeaux-neurocampus.fr/en/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Center+Broca+Nouvelle+Aquitaine/@44.8246349,-0.6079106,15z/data=!4m5!3m4!1s0x0:0x7e5eeebd95bcb30d!8m2!3d44.8246349!4d-0.6079106</t>
+  </si>
+  <si>
+    <t>Marseille</t>
+  </si>
+  <si>
+    <t>INSERM / Aix Marseille University</t>
+  </si>
+  <si>
+    <t>https://ins-amu.fr/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Facult%C3%A9+des+Sciences+M%C3%A9dicales+et+Param%C3%A9dicales+secteur+Timone+(Aix-Marseille+Universit%C3%A9)/@43.2889617,5.3985376,17z/data=!3m1!4b1!4m5!3m4!1s0x12c9bf507bee73e9:0x2471a02cbbd524fe!8m2!3d43.2889617!4d5.4007263</t>
+  </si>
+  <si>
+    <t>INMED/Marseille</t>
+  </si>
+  <si>
+    <t>https://neuro-marseille.org/en/laboratories/mediterranean-neurobiology-institute/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Mediterranean+Institute+of+Neurobiology/@43.2307723,5.4436183,17z/data=!4m12!1m6!3m5!1s0x12c9b9af8fa4e59d:0xf24891781c5cfd74!2sMediterranean+Institute+of+Neurobiology!8m2!3d43.2307684!4d5.445807!3m4!1s0x12c9b9af8fa4e59d:0xf24891781c5cfd74!8m2!3d43.2307684!4d5.445807</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>IPNP Paris</t>
+  </si>
+  <si>
+    <t>https://ipnp.paris5.inserm.fr/research/teams-and-projects</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Center+Psychiatry+Et+Neurosciences/@48.8274506,2.341431,15z/data=!4m2!3m1!1s0x0:0x8f4d2bc12412f5d8?sa=X&amp;ved=2ahUKEwiThd7bpb3vAhXlpIsKHW8BCKIQ_BIwDHoECB8QBQ</t>
+  </si>
+  <si>
+    <t>ENP</t>
+  </si>
+  <si>
+    <t>http://www.paris-neuroscience.fr/en/enp</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/%C3%89cole+des+Neurosciences+de+Paris+%C3%8Ele-de-France/@48.8507603,2.3412757,15z/data=!4m5!3m4!1s0x0:0x121168b4967cfd03!8m2!3d48.8507603!4d2.3412757</t>
+  </si>
+  <si>
+    <t>Universite de Paris</t>
+  </si>
+  <si>
+    <t>https://u-paris.fr/en/master-in-neurosciences/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/University+of+Paris/@48.8553681,2.3316655,15z/data=!4m2!3m1!1s0x0:0xd9bdd83ca3691659?sa=X&amp;ved=2ahUKEwiow9Wy5r_vAhVliYsKHUC1Ci8Q_BIwDXoECBsQBQ</t>
+  </si>
+  <si>
+    <t>Institut Pasteur</t>
+  </si>
+  <si>
+    <t>https://www.pasteur.fr/en/our-missions/research/neuroscience</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Pasteur+Institute/@48.8407721,2.3086963,17z/data=!3m1!4b1!4m5!3m4!1s0x47e670376abf4b5b:0xe831277d10f68655!8m2!3d48.8407686!4d2.310885</t>
+  </si>
+  <si>
+    <t>Institue Neurosciences Cognition</t>
+  </si>
+  <si>
+    <t>https://inc.parisdescartes.fr/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Universit%C3%A9+de+Paris+Campus+-+Saint-Germain-des-Pr%C3%A9s/@48.8549422,2.3268385,15.71z/data=!4m5!3m4!1s0x47e671d7c324482b:0x5cd6e016f2621760!8m2!3d48.8558061!4d2.331577</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Einstein Center Neurosciences</t>
+  </si>
+  <si>
+    <t>https://www.ecn-berlin.de/members/members.html</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Einstein+Center+for+Neurosciences+Berlin/@52.5275686,13.3587414,14z/data=!4m5!3m4!1s0x47a85194e33abec1:0x47c3646428cafdf7!8m2!3d52.5275654!4d13.376251</t>
+  </si>
+  <si>
+    <t>Charite Inst Neurophys</t>
+  </si>
+  <si>
+    <t>https://neurophysiologie.charite.de/en/research/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Charit%C3%A9+-+Universit%C3%A4tsmedizin+Berlin,+Campus+Benjamin+Franklin/@52.4417911,13.2853752,13z/data=!4m5!3m4!1s0x47a85a7d1783705d:0xf6d13a1adcb4376!8m2!3d52.4417879!4d13.3203941</t>
+  </si>
+  <si>
+    <t>Bochum</t>
+  </si>
+  <si>
+    <t>Ruhr University</t>
+  </si>
+  <si>
+    <t>http://www.rd.ruhr-uni-bochum.de/neuro/wiss/index.html.en</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Ruhr-Universit%C3%A4t+Bochum/@51.4456692,7.2265904,13z/data=!4m5!3m4!1s0x47b9203dae9f847b:0x1fb6c82e2deb6a9!8m2!3d51.4456659!4d7.2616093</t>
+  </si>
+  <si>
+    <t>Bonn</t>
+  </si>
+  <si>
+    <t>MP Brain &amp; Behavior</t>
+  </si>
+  <si>
+    <t>https://www.imprs-brain-behavior.org/research/faculty/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/International+Max+Planck+Research+School+(IMPRS)+for+Brain+and+Behavior/@50.7042307,7.1335787,14z/data=!4m5!3m4!1s0x47bee5be14f9174b:0x1d883eecfb2d0470!8m2!3d50.7042273!4d7.1510882</t>
+  </si>
+  <si>
+    <t>Bonn Center of Neuroscience</t>
+  </si>
+  <si>
+    <t>https://bonn-neuroscience.de/bcn-member/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Center+for+Economics+and+Neuroscience/@50.7037044,7.0724915,14z/data=!4m5!3m4!1s0x47bee22df266582f:0x88f8f0bfef31d500!8m2!3d50.703701!4d7.090001</t>
+  </si>
+  <si>
+    <t>Cologne</t>
+  </si>
+  <si>
+    <t>University of Cologne</t>
+  </si>
+  <si>
+    <t>https://zoologie.uni-koeln.de/en/research-divider/neurobiology/neurosciences-in-cologne</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/University+of+Cologne/@50.9281625,6.9288193,15z/data=!4m5!3m4!1s0x0:0x21c4c1ace6430b3c!8m2!3d50.9281625!4d6.9288193</t>
+  </si>
+  <si>
+    <t>Frankfurt</t>
+  </si>
+  <si>
+    <t>MPI</t>
+  </si>
+  <si>
+    <t>https://brain.mpg.de/research.html</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Max-Planck-Institut+f%C3%BCr+Hirnforschung/@50.1455632,8.5996383,13z/data=!4m5!3m4!1s0x41731485013c9783:0xb4349335a84d8d34!8m2!3d50.1742631!4d8.6298507</t>
+  </si>
+  <si>
+    <t>Freiburg</t>
+  </si>
+  <si>
+    <t>Freiburg University</t>
+  </si>
+  <si>
+    <t>https://www.neuro.uni-freiburg.de/institutes</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/University+of+Freiburg/@47.9935477,7.8284401,14z/data=!4m5!3m4!1s0x47911b7d96ce54a1:0x98fcc099eedee1ce!8m2!3d47.9935441!4d7.8459496</t>
+  </si>
+  <si>
+    <t>Goettingen</t>
+  </si>
+  <si>
+    <t>GAU-Goettingen</t>
+  </si>
+  <si>
+    <t>http://www.gpneuro.uni-goettingen.de/content/c_faculty.php</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/University+of+G%C3%B6ttingen/@51.5408149,9.9330231,16z/data=!4m5!3m4!1s0x47a4d4958453d275:0xd273b9e175d47905!8m2!3d51.5408116!4d9.9374004</t>
+  </si>
+  <si>
+    <t>Heidelberg</t>
+  </si>
+  <si>
+    <t>Interdisciplinary Center for Neurosciences</t>
+  </si>
+  <si>
+    <t>https://www.uni-heidelberg.de/izn/ResearchGroups.html</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Heidelberg+University/@49.4191437,8.6352303,13z/data=!4m5!3m4!1s0x4797c106c668f935:0x127da0a49afc15!8m2!3d49.4191402!4d8.6702492</t>
+  </si>
+  <si>
+    <t>Leipzig</t>
+  </si>
+  <si>
+    <t>MPI for Human Cognitive and Brain Sciences</t>
+  </si>
+  <si>
+    <t>https://www.cbs.mpg.de/en</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Max+Planck+Institute+for+Human+Cognitive+and+Brain+Sciences/@51.3349476,12.3867335,17z/data=!3m1!4b1!4m5!3m4!1s0x47a6f83991c1d867:0x2856dce7b35998e4!8m2!3d51.3349443!4d12.3889222</t>
+  </si>
+  <si>
+    <t>Tubingen</t>
+  </si>
+  <si>
+    <t>University Tubingen</t>
+  </si>
+  <si>
+    <t>https://uni-tuebingen.de/en/faculties/faculty-of-science/departments/biology/institutes/neurobiology/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Eberhard+Karls+University+of+T%C3%BCbingen/@48.5294817,9.0262645,14z/data=!4m5!3m4!1s0x4799e4d602c012c3:0xc7d51177246c5b39!8m2!3d48.5294782!4d9.043774</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Reykjavik</t>
+  </si>
+  <si>
+    <t>University of Iceland</t>
+  </si>
+  <si>
+    <t>https://www.hi.is/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/University+of+Iceland+-+Nyi+gardur,+101+Reykjav%C3%ADk,+Iceland/@64.1390289,-21.9492234,16z/data=!4m2!3m1!1s0x48d60b30c8b0c3cd:0xda732d4ddc3e8f35?hl=en-NO&amp;gl=no</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Dublin</t>
+  </si>
+  <si>
+    <t>Trinity College Dublin</t>
+  </si>
+  <si>
+    <t>https://www.tcd.ie/Neuroscience/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Trinity+College+Dublin/@53.3437935,-6.2567603,17z/data=!3m1!4b1!4m5!3m4!1s0x48670e9b2dc78edd:0x2700fe0d8c716167!8m2!3d53.3437935!4d-6.2545716</t>
+  </si>
+  <si>
     <t>Netherlands</t>
   </si>
   <si>
@@ -470,6 +824,15 @@
     <t>https://www.google.com/maps/place/Netherlands+Institute+for+Neuroscience/@52.3051753,4.9181704,13.12z/data=!4m5!3m4!1s0x47c60b7c53416347:0xdb9ff64c4aa64389!8m2!3d52.2924742!4d4.9575557</t>
   </si>
   <si>
+    <t>Vrije Universiteit Amsterdam</t>
+  </si>
+  <si>
+    <t>https://vuweb.vu.nl/en/education/master/neurosciences</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Vrije+Universiteit+Amsterdam/@52.3337601,4.8635312,17z/data=!3m1!4b1!4m5!3m4!1s0x47c60a085c443af1:0x2df2d7a997eccd84!8m2!3d52.3337568!4d4.8657199</t>
+  </si>
+  <si>
     <t>Leiden</t>
   </si>
   <si>
@@ -482,6 +845,30 @@
     <t>https://www.google.com/maps/place/Leiden+University/@52.1576673,4.477487,15.23z/data=!4m5!3m4!1s0x47c5c6f2447daae3:0x48e9dc4f075bb167!8m2!3d52.1571485!4d4.485209</t>
   </si>
   <si>
+    <t>Nijmegen</t>
+  </si>
+  <si>
+    <t>Donders Institute</t>
+  </si>
+  <si>
+    <t>https://www.ru.nl/donders/research/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Donders+Centre+for+Cognition/@51.8227138,5.8571355,16z/data=!4m8!1m2!2m1!1sdonders+radboud!3m4!1s0x47c708eeef1a7ddf:0x3383a57205a4a83e!8m2!3d51.8193166!4d5.8596925</t>
+  </si>
+  <si>
+    <t>Rotterdam</t>
+  </si>
+  <si>
+    <t>Erasmus MC</t>
+  </si>
+  <si>
+    <t>https://neuro.nl/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Erasmus+University+Medical+Center/@51.9141188,4.4605011,13z/data=!4m8!1m2!2m1!1srotterdam+neuroscience!3m4!1s0x47c4349bd0000001:0x8491118325eb0fe6!8m2!3d51.9108848!4d4.4678541</t>
+  </si>
+  <si>
     <t>Utrecht</t>
   </si>
   <si>
@@ -494,150 +881,57 @@
     <t>https://www.google.com/maps/place/Neuroscience+%26+Cognition/@52.0884921,5.1087716,13z/data=!4m8!1m2!2m1!1sutrecht+neuroscience!3m4!1s0x47c6688517970ef7:0xf19ed5f79cd67ad6!8m2!3d52.0864602!4d5.1767407</t>
   </si>
   <si>
-    <t>Nijmegen</t>
-  </si>
-  <si>
-    <t>Donders Institute</t>
-  </si>
-  <si>
-    <t>https://www.ru.nl/donders/research/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Donders+Centre+for+Cognition/@51.8227138,5.8571355,16z/data=!4m8!1m2!2m1!1sdonders+radboud!3m4!1s0x47c708eeef1a7ddf:0x3383a57205a4a83e!8m2!3d51.8193166!4d5.8596925</t>
-  </si>
-  <si>
-    <t>Rotterdam</t>
-  </si>
-  <si>
-    <t>Erasmus MC</t>
-  </si>
-  <si>
-    <t>https://neuro.nl/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Erasmus+University+Medical+Center/@51.9141188,4.4605011,13z/data=!4m8!1m2!2m1!1srotterdam+neuroscience!3m4!1s0x47c4349bd0000001:0x8491118325eb0fe6!8m2!3d51.9108848!4d4.4678541</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>Berlin</t>
-  </si>
-  <si>
-    <t>Einstein Center Neurosciences</t>
-  </si>
-  <si>
-    <t>https://www.ecn-berlin.de/members/members.html</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Einstein+Center+for+Neurosciences+Berlin/@52.5275686,13.3587414,14z/data=!4m5!3m4!1s0x47a85194e33abec1:0x47c3646428cafdf7!8m2!3d52.5275654!4d13.376251</t>
-  </si>
-  <si>
-    <t>Charite Inst Neurophys</t>
-  </si>
-  <si>
-    <t>https://neurophysiologie.charite.de/en/research/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Charit%C3%A9+-+Universit%C3%A4tsmedizin+Berlin,+Campus+Benjamin+Franklin/@52.4417911,13.2853752,13z/data=!4m5!3m4!1s0x47a85a7d1783705d:0xf6d13a1adcb4376!8m2!3d52.4417879!4d13.3203941</t>
-  </si>
-  <si>
-    <t>Goettingen</t>
-  </si>
-  <si>
-    <t>GAU-Goettingen</t>
-  </si>
-  <si>
-    <t>http://www.gpneuro.uni-goettingen.de/content/c_faculty.php</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/University+of+G%C3%B6ttingen/@51.5408149,9.9330231,16z/data=!4m5!3m4!1s0x47a4d4958453d275:0xd273b9e175d47905!8m2!3d51.5408116!4d9.9374004</t>
-  </si>
-  <si>
-    <t>Tubingen</t>
-  </si>
-  <si>
-    <t>University Tubingen</t>
-  </si>
-  <si>
-    <t>https://uni-tuebingen.de/en/faculties/faculty-of-science/departments/biology/institutes/neurobiology/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Eberhard+Karls+University+of+T%C3%BCbingen/@48.5294817,9.0262645,14z/data=!4m5!3m4!1s0x4799e4d602c012c3:0xc7d51177246c5b39!8m2!3d48.5294782!4d9.043774</t>
-  </si>
-  <si>
-    <t>Heidelberg</t>
-  </si>
-  <si>
-    <t>Interdisciplinary Center for Neurosciences</t>
-  </si>
-  <si>
-    <t>https://www.uni-heidelberg.de/izn/ResearchGroups.html</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Heidelberg+University/@49.4191437,8.6352303,13z/data=!4m5!3m4!1s0x4797c106c668f935:0x127da0a49afc15!8m2!3d49.4191402!4d8.6702492</t>
-  </si>
-  <si>
-    <t>Freiburg</t>
-  </si>
-  <si>
-    <t>Freiburg University</t>
-  </si>
-  <si>
-    <t>https://www.neuro.uni-freiburg.de/institutes</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/University+of+Freiburg/@47.9935477,7.8284401,14z/data=!4m5!3m4!1s0x47911b7d96ce54a1:0x98fcc099eedee1ce!8m2!3d47.9935441!4d7.8459496</t>
-  </si>
-  <si>
-    <t>Frankfurt</t>
-  </si>
-  <si>
-    <t>MPI</t>
-  </si>
-  <si>
-    <t>https://brain.mpg.de/research.html</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Max-Planck-Institut+f%C3%BCr+Hirnforschung/@50.1455632,8.5996383,13z/data=!4m5!3m4!1s0x41731485013c9783:0xb4349335a84d8d34!8m2!3d50.1742631!4d8.6298507</t>
-  </si>
-  <si>
-    <t>Bonn</t>
-  </si>
-  <si>
-    <t>MP Brain &amp; Behavior</t>
-  </si>
-  <si>
-    <t>https://www.imprs-brain-behavior.org/research/faculty/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/International+Max+Planck+Research+School+(IMPRS)+for+Brain+and+Behavior/@50.7042307,7.1335787,14z/data=!4m5!3m4!1s0x47bee5be14f9174b:0x1d883eecfb2d0470!8m2!3d50.7042273!4d7.1510882</t>
-  </si>
-  <si>
-    <t>Bonn Center of Neuroscience</t>
-  </si>
-  <si>
-    <t>https://bonn-neuroscience.de/bcn-member/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Center+for+Economics+and+Neuroscience/@50.7037044,7.0724915,14z/data=!4m5!3m4!1s0x47bee22df266582f:0x88f8f0bfef31d500!8m2!3d50.703701!4d7.090001</t>
-  </si>
-  <si>
-    <t>Bochum</t>
-  </si>
-  <si>
-    <t>Ruhr University</t>
-  </si>
-  <si>
-    <t>http://www.rd.ruhr-uni-bochum.de/neuro/wiss/index.html.en</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Ruhr-Universit%C3%A4t+Bochum/@51.4456692,7.2265904,13z/data=!4m5!3m4!1s0x47b9203dae9f847b:0x1fb6c82e2deb6a9!8m2!3d51.4456659!4d7.2616093</t>
+    <t>Scotland</t>
+  </si>
+  <si>
+    <t>Edinburgh</t>
+  </si>
+  <si>
+    <t>University of Edinburgh</t>
+  </si>
+  <si>
+    <t>https://www.edinburghneuroscience.ed.ac.uk/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/The+University+of+Edinburgh/@55.9445118,-3.1908205,17z/data=!4m8!1m2!2m1!1suniversity+of+edinburgh+neuroscience+phd!3m4!1s0x4887c786156c3b5d:0xb21928d390bbc0ee!8m2!3d55.9445158!4d-3.1892413</t>
   </si>
   <si>
     <t>Switzerland</t>
   </si>
   <si>
+    <t>Basel</t>
+  </si>
+  <si>
+    <t>Biozentrum University of Basel</t>
+  </si>
+  <si>
+    <t>https://www.biozentrum.unibas.ch/research/researchgroups/research-areas/neurobiology/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Biozentrum+University+of+Basel/@47.5639238,7.5624544,14z/data=!4m5!3m4!1s0x4791b908135df8df:0x850b8df911af1a74!8m2!3d47.5639202!4d7.5799639</t>
+  </si>
+  <si>
+    <t>FMI</t>
+  </si>
+  <si>
+    <t>https://www.fmi.ch/research-groups/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Friedrich+Miescher+Institute+for+Biomedical+Research+(FMI)/@47.5677684,7.5862484,14z/data=!4m8!1m2!2m1!1sfmi+neuroscience!3m4!1s0x4791b9bf1ea23113:0xe62d992342b87bd9!8m2!3d47.5677684!4d7.6037579</t>
+  </si>
+  <si>
+    <t>Lausanne</t>
+  </si>
+  <si>
+    <t>EPFL</t>
+  </si>
+  <si>
+    <t>https://www.epfl.ch/schools/sv/bmi/brain-mind-institute/epfl-neuro-research-groups/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/EPFL,+1015+Lausanne,+Switzerland/@46.5189902,6.5500912,14z/data=!4m5!3m4!1s0x478c30fe7ab739e3:0x6051b4607fcb144a!8m2!3d46.5189865!4d6.5676007</t>
+  </si>
+  <si>
     <t>Zurich</t>
   </si>
   <si>
@@ -650,285 +944,6 @@
     <t>https://www.google.com/maps/place/University+of+Zurich/@47.3743257,8.5422265,15z/data=!4m5!3m4!1s0x479aa09f5895858b:0xba50fa52d07edacf!8m2!3d47.3743221!4d8.5509812</t>
   </si>
   <si>
-    <t>Basel</t>
-  </si>
-  <si>
-    <t>Biozentrum University of Basel</t>
-  </si>
-  <si>
-    <t>https://www.biozentrum.unibas.ch/research/researchgroups/research-areas/neurobiology/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Biozentrum+University+of+Basel/@47.5639238,7.5624544,14z/data=!4m5!3m4!1s0x4791b908135df8df:0x850b8df911af1a74!8m2!3d47.5639202!4d7.5799639</t>
-  </si>
-  <si>
-    <t>FMI</t>
-  </si>
-  <si>
-    <t>https://www.fmi.ch/research-groups/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Friedrich+Miescher+Institute+for+Biomedical+Research+(FMI)/@47.5677684,7.5862484,14z/data=!4m8!1m2!2m1!1sfmi+neuroscience!3m4!1s0x4791b9bf1ea23113:0xe62d992342b87bd9!8m2!3d47.5677684!4d7.6037579</t>
-  </si>
-  <si>
-    <t>Lausanne</t>
-  </si>
-  <si>
-    <t>EPFL</t>
-  </si>
-  <si>
-    <t>https://www.epfl.ch/schools/sv/bmi/brain-mind-institute/epfl-neuro-research-groups/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/EPFL,+1015+Lausanne,+Switzerland/@46.5189902,6.5500912,14z/data=!4m5!3m4!1s0x478c30fe7ab739e3:0x6051b4607fcb144a!8m2!3d46.5189865!4d6.5676007</t>
-  </si>
-  <si>
-    <t>Cologne</t>
-  </si>
-  <si>
-    <t>University of Cologne</t>
-  </si>
-  <si>
-    <t>https://zoologie.uni-koeln.de/en/research-divider/neurobiology/neurosciences-in-cologne</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/University+of+Cologne/@50.9281625,6.9288193,15z/data=!4m5!3m4!1s0x0:0x21c4c1ace6430b3c!8m2!3d50.9281625!4d6.9288193</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Marseille</t>
-  </si>
-  <si>
-    <t>INSERM / Aix Marseille University</t>
-  </si>
-  <si>
-    <t>https://ins-amu.fr/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Facult%C3%A9+des+Sciences+M%C3%A9dicales+et+Param%C3%A9dicales+secteur+Timone+(Aix-Marseille+Universit%C3%A9)/@43.2889617,5.3985376,17z/data=!3m1!4b1!4m5!3m4!1s0x12c9bf507bee73e9:0x2471a02cbbd524fe!8m2!3d43.2889617!4d5.4007263</t>
-  </si>
-  <si>
-    <t>Vrije Universiteit Amsterdam</t>
-  </si>
-  <si>
-    <t>https://vuweb.vu.nl/en/education/master/neurosciences</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Vrije+Universiteit+Amsterdam/@52.3337601,4.8635312,17z/data=!3m1!4b1!4m5!3m4!1s0x47c60a085c443af1:0x2df2d7a997eccd84!8m2!3d52.3337568!4d4.8657199</t>
-  </si>
-  <si>
-    <t>Paris</t>
-  </si>
-  <si>
-    <t>IPNP Paris</t>
-  </si>
-  <si>
-    <t>https://ipnp.paris5.inserm.fr/research/teams-and-projects</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Center+Psychiatry+Et+Neurosciences/@48.8274506,2.341431,15z/data=!4m2!3m1!1s0x0:0x8f4d2bc12412f5d8?sa=X&amp;ved=2ahUKEwiThd7bpb3vAhXlpIsKHW8BCKIQ_BIwDHoECB8QBQ</t>
-  </si>
-  <si>
-    <t>INMED/Marseille</t>
-  </si>
-  <si>
-    <t>https://neuro-marseille.org/en/laboratories/mediterranean-neurobiology-institute/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Mediterranean+Institute+of+Neurobiology/@43.2307723,5.4436183,17z/data=!4m12!1m6!3m5!1s0x12c9b9af8fa4e59d:0xf24891781c5cfd74!2sMediterranean+Institute+of+Neurobiology!8m2!3d43.2307684!4d5.445807!3m4!1s0x12c9b9af8fa4e59d:0xf24891781c5cfd74!8m2!3d43.2307684!4d5.445807</t>
-  </si>
-  <si>
-    <t>England</t>
-  </si>
-  <si>
-    <t>London</t>
-  </si>
-  <si>
-    <t>King's College</t>
-  </si>
-  <si>
-    <t>https://www.kcl.ac.uk/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/King's+College+London/@51.5114864,-0.115997,15z/data=!4m5!3m4!1s0x0:0xb0643efb7ed0928d!8m2!3d51.5114864!4d-0.115997</t>
-  </si>
-  <si>
-    <t>Cambridge</t>
-  </si>
-  <si>
-    <t>University of Cambridge</t>
-  </si>
-  <si>
-    <t>http://www.cam.ac.uk/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/University+of+Cambridge/@52.2042666,0.1149085,15z/data=!4m5!3m4!1s0x0:0x21ca80abf36db5bb!8m2!3d52.2042666!4d0.1149085</t>
-  </si>
-  <si>
-    <t>Oxford</t>
-  </si>
-  <si>
-    <t>University of Oxford</t>
-  </si>
-  <si>
-    <t>https://www.neuroscience.ox.ac.uk/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/University+of+Oxford/@51.710979,-1.3093672,12z/data=!4m8!1m2!2m1!1soxford+neuroscience!3m4!1s0x4876c6a9ef8c485b:0xd2ff1883a001afed!8m2!3d51.7548164!4d-1.2543668</t>
-  </si>
-  <si>
-    <t>UCL</t>
-  </si>
-  <si>
-    <t>https://www.ucl.ac.uk/research/domains/neuroscience</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/UCL+Institute+of+Cognitive+Neuroscience/@51.5221999,-0.1254988,17z/data=!3m1!4b1!4m5!3m4!1s0x48761b36ce873581:0xa29303ad768432d5!8m2!3d51.5221999!4d-0.1233101</t>
-  </si>
-  <si>
-    <t>Scotland</t>
-  </si>
-  <si>
-    <t>Edinburgh</t>
-  </si>
-  <si>
-    <t>University of Edinburgh</t>
-  </si>
-  <si>
-    <t>https://www.edinburghneuroscience.ed.ac.uk/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/The+University+of+Edinburgh/@55.9445118,-3.1908205,17z/data=!4m8!1m2!2m1!1suniversity+of+edinburgh+neuroscience+phd!3m4!1s0x4887c786156c3b5d:0xb21928d390bbc0ee!8m2!3d55.9445158!4d-3.1892413</t>
-  </si>
-  <si>
-    <t>Ireland</t>
-  </si>
-  <si>
-    <t>Dublin</t>
-  </si>
-  <si>
-    <t>Trinity College Dublin</t>
-  </si>
-  <si>
-    <t>https://www.tcd.ie/Neuroscience/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Trinity+College+Dublin/@53.3437935,-6.2567603,17z/data=!3m1!4b1!4m5!3m4!1s0x48670e9b2dc78edd:0x2700fe0d8c716167!8m2!3d53.3437935!4d-6.2545716</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>Leuven</t>
-  </si>
-  <si>
-    <t>KU Leuven</t>
-  </si>
-  <si>
-    <t>https://www.kuleuven.be/kuleuven/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Katholieke+Universiteit+Leuven/@50.8779545,4.7002953,15z/data=!4m5!3m4!1s0x0:0x2cf72ac3db15442d!8m2!3d50.8779545!4d4.7002953</t>
-  </si>
-  <si>
-    <t>Leipzig</t>
-  </si>
-  <si>
-    <t>MPI for Human Cognitive and Brain Sciences</t>
-  </si>
-  <si>
-    <t>https://www.cbs.mpg.de/en</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Max+Planck+Institute+for+Human+Cognitive+and+Brain+Sciences/@51.3349476,12.3867335,17z/data=!3m1!4b1!4m5!3m4!1s0x47a6f83991c1d867:0x2856dce7b35998e4!8m2!3d51.3349443!4d12.3889222</t>
-  </si>
-  <si>
-    <t>Brussels</t>
-  </si>
-  <si>
-    <t>ULB Neuroscience Institute</t>
-  </si>
-  <si>
-    <t>https://uni.ulb.ac.be/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Universit%C3%A9+Libre+de+Bruxelles/@50.8132102,4.3800335,17z/data=!3m1!4b1!4m5!3m4!1s0x47c3c4485d19ce43:0xe8eb9253c07c6691!8m2!3d50.8132068!4d4.3822222</t>
-  </si>
-  <si>
-    <t>Bordeaux</t>
-  </si>
-  <si>
-    <t>Bordeaux Neurocampus</t>
-  </si>
-  <si>
-    <t>https://www.bordeaux-neurocampus.fr/en/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Center+Broca+Nouvelle+Aquitaine/@44.8246349,-0.6079106,15z/data=!4m5!3m4!1s0x0:0x7e5eeebd95bcb30d!8m2!3d44.8246349!4d-0.6079106</t>
-  </si>
-  <si>
-    <t>ENP</t>
-  </si>
-  <si>
-    <t>http://www.paris-neuroscience.fr/en/enp</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/%C3%89cole+des+Neurosciences+de+Paris+%C3%8Ele-de-France/@48.8507603,2.3412757,15z/data=!4m5!3m4!1s0x0:0x121168b4967cfd03!8m2!3d48.8507603!4d2.3412757</t>
-  </si>
-  <si>
-    <t>Universite de Paris</t>
-  </si>
-  <si>
-    <t>https://u-paris.fr/en/master-in-neurosciences/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/University+of+Paris/@48.8553681,2.3316655,15z/data=!4m2!3m1!1s0x0:0xd9bdd83ca3691659?sa=X&amp;ved=2ahUKEwiow9Wy5r_vAhVliYsKHUC1Ci8Q_BIwDXoECBsQBQ</t>
-  </si>
-  <si>
-    <t>Institut Pasteur</t>
-  </si>
-  <si>
-    <t>https://www.pasteur.fr/en/our-missions/research/neuroscience</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Pasteur+Institute/@48.8407721,2.3086963,17z/data=!3m1!4b1!4m5!3m4!1s0x47e670376abf4b5b:0xe831277d10f68655!8m2!3d48.8407686!4d2.310885</t>
-  </si>
-  <si>
-    <t>Institue Neurosciences Cognition</t>
-  </si>
-  <si>
-    <t>https://inc.parisdescartes.fr/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Universit%C3%A9+de+Paris+Campus+-+Saint-Germain-des-Pr%C3%A9s/@48.8549422,2.3268385,15.71z/data=!4m5!3m4!1s0x47e671d7c324482b:0x5cd6e016f2621760!8m2!3d48.8558061!4d2.331577</t>
-  </si>
-  <si>
-    <t>Cardiff</t>
-  </si>
-  <si>
-    <t>Cardiff University</t>
-  </si>
-  <si>
-    <t>https://www.cardiff.ac.uk/neuroscience-mental-health/research</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Cardiff+University/@51.4814204,-3.184425,14.41z/data=!4m8!1m2!2m1!1scardiff+neuroscience!3m4!1s0x0:0xe06dc7099e7122ca!8m2!3d51.4866276!4d-3.1788683</t>
-  </si>
-  <si>
-    <t>Bristol</t>
-  </si>
-  <si>
-    <t>University of Bristol</t>
-  </si>
-  <si>
-    <t>http://www.bristol.ac.uk/neuroscience/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/University+of+Bristol/@51.4584074,-2.6037595,18.18z/data=!4m5!3m4!1s0x48718ddbdfd292fb:0x2f0b60f89b4b6d56!8m2!3d51.4584172!4d-2.6029792</t>
-  </si>
-  <si>
     <t>Wales</t>
   </si>
   <si>
@@ -950,6 +965,27 @@
     <t>Canada</t>
   </si>
   <si>
+    <t>Lethbridge</t>
+  </si>
+  <si>
+    <t>University of Lethbridge</t>
+  </si>
+  <si>
+    <t>https://www.uleth.ca/artsci/neuroscience</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Canadian+Center+for+Behavioral+Neuroscience/@49.6807166,-112.8684929,15z/data=!4m5!3m4!1s0x0:0x4ed1cfad4b7484f2!8m2!3d49.6807166!4d-112.8684929</t>
+  </si>
+  <si>
+    <t>Western University</t>
+  </si>
+  <si>
+    <t>https://www.schulich.uwo.ca/neuroscience/graduate/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Western+University/@43.0087011,-81.2773704,16z/data=!4m8!1m2!2m1!1swestern+university+neuroscience!3m4!1s0x882eee0e6ac42bd1:0xaa87f353aab9799b!8m2!3d43.0095971!4d-81.2737336</t>
+  </si>
+  <si>
     <t>Montreal</t>
   </si>
   <si>
@@ -962,13 +998,37 @@
     <t>https://www.google.com/maps/place/Montreal+Neurological+Institute+and+Hospital/@45.5089963,-73.5813729,15z/data=!4m2!3m1!1s0x0:0xd75187e12c47cf1c?sa=X&amp;ved=2ahUKEwjY9_Dz3L7vAhVxwosKHYsVDMUQ_BIwEnoECCQQBQ</t>
   </si>
   <si>
-    <t>Western University</t>
-  </si>
-  <si>
-    <t>https://www.schulich.uwo.ca/neuroscience/graduate/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Western+University/@43.0087011,-81.2773704,16z/data=!4m8!1m2!2m1!1swestern+university+neuroscience!3m4!1s0x882eee0e6ac42bd1:0xaa87f353aab9799b!8m2!3d43.0095971!4d-81.2737336</t>
+    <t>Quebec City</t>
+  </si>
+  <si>
+    <t>Universite Laval</t>
+  </si>
+  <si>
+    <t>https://neuro.ulaval.ca/en</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Laval+University/@46.7817463,-71.2769311,17z/data=!3m1!4b1!4m5!3m4!1s0x4cb896c469ff32f9:0x15feb853bd2f8247!8m2!3d46.7817463!4d-71.2747424</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Unversity of Toronto</t>
+  </si>
+  <si>
+    <t>http://www.neuroscience.utoronto.ca/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/University+of+Toronto+-+St.+George+Campus/@43.6638108,-79.4005143,17z/data=!4m8!1m2!2m1!1suniversity+of+toronto+neuroscience!3m4!1s0x882b34b8f331fd9b:0x8d1d9bb6765a76f7!8m2!3d43.6628917!4d-79.3956564</t>
+  </si>
+  <si>
+    <t>SickKids NMH</t>
+  </si>
+  <si>
+    <t>https://www.sickkids.ca/en/research/research-programs/neurosciences-mental-health/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/The+Hospital+for+Sick+Children/@43.6573235,-79.3894919,17z/data=!3m1!4b1!4m5!3m4!1s0x882b34c9b2253cc9:0xd626f96dbbd306cf!8m2!3d43.6573235!4d-79.3873032</t>
   </si>
   <si>
     <t>Vancouver</t>
@@ -983,30 +1043,69 @@
     <t>https://www.google.com/maps/place/The+University+of+British+Columbia/@49.2625228,-123.2536585,16z/data=!4m8!1m2!2m1!1subc+neuroscience!3m4!1s0x548672cc2fd41e03:0xc79dd4e7732aa2f3!8m2!3d49.2606052!4d-123.2459938</t>
   </si>
   <si>
-    <t>Toronto</t>
-  </si>
-  <si>
-    <t>Unversity of Toronto</t>
-  </si>
-  <si>
-    <t>http://www.neuroscience.utoronto.ca/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/University+of+Toronto+-+St.+George+Campus/@43.6638108,-79.4005143,17z/data=!4m8!1m2!2m1!1suniversity+of+toronto+neuroscience!3m4!1s0x882b34b8f331fd9b:0x8d1d9bb6765a76f7!8m2!3d43.6628917!4d-79.3956564</t>
-  </si>
-  <si>
-    <t>SickKids NMH</t>
-  </si>
-  <si>
-    <t>https://www.sickkids.ca/en/research/research-programs/neurosciences-mental-health/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/The+Hospital+for+Sick+Children/@43.6573235,-79.3894919,17z/data=!3m1!4b1!4m5!3m4!1s0x882b34c9b2253cc9:0xd626f96dbbd306cf!8m2!3d43.6573235!4d-79.3873032</t>
-  </si>
-  <si>
     <t>USA</t>
   </si>
   <si>
+    <t>Ashburn</t>
+  </si>
+  <si>
+    <t>Janelia Research Campus</t>
+  </si>
+  <si>
+    <t>https://www.janelia.org/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Janelia+Research+Campus/@39.0714096,-77.4642701,15z/data=!4m5!3m4!1s0x0:0x86d91f3d79ea0884!8m2!3d39.0714096!4d-77.4642701</t>
+  </si>
+  <si>
+    <t>Cold Spring Harbor</t>
+  </si>
+  <si>
+    <t>Cold Spring Harbor Laboratory</t>
+  </si>
+  <si>
+    <t>https://www.cshl.edu/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Cold+Spring+Harbor+Laboratory/@40.8580545,-73.4669315,15z/data=!4m5!3m4!1s0x0:0xfcd58807ef419c9a!8m2!3d40.8580545!4d-73.4669315</t>
+  </si>
+  <si>
+    <t>Jupiter</t>
+  </si>
+  <si>
+    <t>Max Planck Florida Institute for Neuroscience</t>
+  </si>
+  <si>
+    <t>https://mpfi.org/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Max+Planck+Florida+Institute+for+Neuroscience/@26.8838274,-80.1170496,17z/data=!3m1!4b1!4m5!3m4!1s0x88ded5be31da3a65:0x93ddb5033354d5c8!8m2!3d26.8838274!4d-80.1148609</t>
+  </si>
+  <si>
+    <t>Rockville</t>
+  </si>
+  <si>
+    <t>NIH</t>
+  </si>
+  <si>
+    <t>https://dir.ninds.nih.gov/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/National+Institutes+of+Health/@39.0503293,-77.1228336,17z/data=!3m1!4b1!4m5!3m4!1s0x89b7cc39feb1f81d:0x23dee637adc1ff88!8m2!3d39.0503293!4d-77.1206449</t>
+  </si>
+  <si>
+    <t>San Diego</t>
+  </si>
+  <si>
+    <t>Scripps Research Institute</t>
+  </si>
+  <si>
+    <t>https://www.scripps.edu/science-and-medicine/research-departments/neuroscience/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Dorris+Neuroscience+Center+(DNC),+The+Scripps+Research+Institute/@32.8945205,-117.2399002,17z/data=!3m1!4b1!4m5!3m4!1s0x80dc06ee05421e91:0x30fe2adb5283df19!8m2!3d32.8945205!4d-117.2377115</t>
+  </si>
+  <si>
     <t>Seattle</t>
   </si>
   <si>
@@ -1019,96 +1118,24 @@
     <t>https://www.google.com/maps/place/Allen+Institute/@47.6251409,-122.3417072,17z/data=!3m1!4b1!4m5!3m4!1s0x5490150705cb5703:0x499c58d72a7bcf9!8m2!3d47.6251409!4d-122.3395185</t>
   </si>
   <si>
-    <t>Rockville</t>
-  </si>
-  <si>
-    <t>NIH</t>
-  </si>
-  <si>
-    <t>https://dir.ninds.nih.gov/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/National+Institutes+of+Health/@39.0503293,-77.1228336,17z/data=!3m1!4b1!4m5!3m4!1s0x89b7cc39feb1f81d:0x23dee637adc1ff88!8m2!3d39.0503293!4d-77.1206449</t>
-  </si>
-  <si>
-    <t>Ashburn</t>
-  </si>
-  <si>
-    <t>Janelia Research Campus</t>
-  </si>
-  <si>
-    <t>https://www.janelia.org/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Janelia+Research+Campus/@39.0714096,-77.4642701,15z/data=!4m5!3m4!1s0x0:0x86d91f3d79ea0884!8m2!3d39.0714096!4d-77.4642701</t>
-  </si>
-  <si>
-    <t>Jupiter</t>
-  </si>
-  <si>
-    <t>Max Planck Florida Institute for Neuroscience</t>
-  </si>
-  <si>
-    <t>https://mpfi.org/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Max+Planck+Florida+Institute+for+Neuroscience/@26.8838274,-80.1170496,17z/data=!3m1!4b1!4m5!3m4!1s0x88ded5be31da3a65:0x93ddb5033354d5c8!8m2!3d26.8838274!4d-80.1148609</t>
-  </si>
-  <si>
-    <t>San Diego</t>
-  </si>
-  <si>
-    <t>Scripps Research Institute</t>
-  </si>
-  <si>
-    <t>https://www.scripps.edu/science-and-medicine/research-departments/neuroscience/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Dorris+Neuroscience+Center+(DNC),+The+Scripps+Research+Institute/@32.8945205,-117.2399002,17z/data=!3m1!4b1!4m5!3m4!1s0x80dc06ee05421e91:0x30fe2adb5283df19!8m2!3d32.8945205!4d-117.2377115</t>
-  </si>
-  <si>
-    <t>Lethbridge</t>
-  </si>
-  <si>
-    <t>University of Lethbridge</t>
-  </si>
-  <si>
-    <t>https://www.uleth.ca/artsci/neuroscience</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Canadian+Center+for+Behavioral+Neuroscience/@49.6807166,-112.8684929,15z/data=!4m5!3m4!1s0x0:0x4ed1cfad4b7484f2!8m2!3d49.6807166!4d-112.8684929</t>
-  </si>
-  <si>
-    <t>Cold Spring Harbor</t>
-  </si>
-  <si>
-    <t>Cold Spring Harbor Laboratory</t>
-  </si>
-  <si>
-    <t>https://www.cshl.edu/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Cold+Spring+Harbor+Laboratory/@40.8580545,-73.4669315,15z/data=!4m5!3m4!1s0x0:0xfcd58807ef419c9a!8m2!3d40.8580545!4d-73.4669315</t>
-  </si>
-  <si>
-    <t>Quebec City</t>
-  </si>
-  <si>
-    <t>Universite Laval</t>
-  </si>
-  <si>
-    <t>https://neuro.ulaval.ca/en</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/Laval+University/@46.7817463,-71.2769311,17z/data=!3m1!4b1!4m5!3m4!1s0x4cb896c469ff32f9:0x15feb853bd2f8247!8m2!3d46.7817463!4d-71.2747424</t>
-  </si>
-  <si>
     <t>Oceania</t>
   </si>
   <si>
     <t>Australia</t>
   </si>
   <si>
+    <t>Brisbane</t>
+  </si>
+  <si>
+    <t>University of Queensland Australia</t>
+  </si>
+  <si>
+    <t>https://qbi.uq.edu.au/</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/The+University+of+Queensland/@-27.497498,153.0115018,17z/data=!3m1!4b1!4m5!3m4!1s0x6b91508241eb7c49:0x9ae9946d3710eee9!8m2!3d-27.4975028!4d153.0136905</t>
+  </si>
+  <si>
     <t>Melbourne</t>
   </si>
   <si>
@@ -1133,21 +1160,21 @@
     <t>https://www.google.com/maps/place/Brain+and+Mind+Centre/@-33.8890697,151.1763526,17z/data=!4m8!1m2!2m1!1shttps:%2F%2Fwww.sydney.edu.au%2Fbrain-mind%2F!3m4!1s0x6b12b02f077dff6f:0xeb68c38ffc383072!8m2!3d-33.8885047!4d151.1775438</t>
   </si>
   <si>
-    <t>Brisbane</t>
-  </si>
-  <si>
-    <t>University of Queensland Australia</t>
-  </si>
-  <si>
-    <t>https://qbi.uq.edu.au/</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/The+University+of+Queensland/@-27.497498,153.0115018,17z/data=!3m1!4b1!4m5!3m4!1s0x6b91508241eb7c49:0x9ae9946d3710eee9!8m2!3d-27.4975028!4d153.0136905</t>
-  </si>
-  <si>
     <t>New Zealand</t>
   </si>
   <si>
+    <t>Auckland</t>
+  </si>
+  <si>
+    <t>Unversity of Auckland</t>
+  </si>
+  <si>
+    <t>https://www.auckland.ac.nz/en/study/study-options/find-a-study-option/biomedical-science/undergraduate/bsc-biomedical-from-2019/neuroscience.html</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/The+University+of+Auckland/@-36.8523335,174.7669186,17z/data=!3m1!4b1!4m5!3m4!1s0x6d0d47e383f32253:0xbd49f61f758a9e5b!8m2!3d-36.8523378!4d174.7691073</t>
+  </si>
+  <si>
     <t>Dunedin</t>
   </si>
   <si>
@@ -1158,18 +1185,6 @@
   </si>
   <si>
     <t>https://www.google.com/maps/place/University+of+Otago/@-45.8646835,170.512234,17z/data=!3m1!4b1!4m5!3m4!1s0xa82eac692eec734d:0x761f754c6bfb9a70!8m2!3d-45.8646835!4d170.5144227</t>
-  </si>
-  <si>
-    <t>Auckland</t>
-  </si>
-  <si>
-    <t>Unversity of Auckland</t>
-  </si>
-  <si>
-    <t>https://www.auckland.ac.nz/en/study/study-options/find-a-study-option/biomedical-science/undergraduate/bsc-biomedical-from-2019/neuroscience.html</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/The+University+of+Auckland/@-36.8523335,174.7669186,17z/data=!3m1!4b1!4m5!3m4!1s0x6d0d47e383f32253:0xbd49f61f758a9e5b!8m2!3d-36.8523378!4d174.7691073</t>
   </si>
   <si>
     <t>Singapore</t>
@@ -1286,11 +1301,11 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
-    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -1343,22 +1358,22 @@
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1577,7 +1592,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
@@ -1639,7 +1657,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="4">
-        <v>1450000.0</v>
+        <v>2.1E7</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>10</v>
@@ -1680,7 +1698,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="4">
-        <v>1091000.0</v>
+        <v>2.1E7</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
@@ -1721,9 +1739,9 @@
         <v>17</v>
       </c>
       <c r="D4" s="4">
-        <v>1.3960236E7</v>
-      </c>
-      <c r="E4" s="3" t="s">
+        <v>2.448E7</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -1756,22 +1774,22 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="4">
+        <v>1.1E7</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="4">
-        <v>9700000.0</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -1797,22 +1815,22 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="4">
+        <v>1450000.0</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="4">
-        <v>2.1E7</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -1838,22 +1856,22 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1091000.0</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="4">
-        <v>2.448E7</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -1879,22 +1897,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.3960236E7</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="4">
-        <v>2.1E7</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -1920,15 +1938,15 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="4">
-        <v>1.1E7</v>
-      </c>
-      <c r="E9" s="7" t="s">
+        <v>9700000.0</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -1967,7 +1985,7 @@
         <v>45</v>
       </c>
       <c r="D10" s="4">
-        <v>1.485E7</v>
+        <v>8444000.0</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>46</v>
@@ -2008,7 +2026,7 @@
         <v>49</v>
       </c>
       <c r="D11" s="4">
-        <v>8444000.0</v>
+        <v>1.485E7</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>50</v>
@@ -2171,16 +2189,16 @@
       <c r="C15" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="10">
-        <v>182000.0</v>
+      <c r="D15" s="4">
+        <v>350000.0</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="10" t="s">
         <v>75</v>
       </c>
       <c r="H15" s="6"/>
@@ -2212,16 +2230,16 @@
       <c r="C16" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="10">
-        <v>693000.0</v>
+      <c r="D16" s="4">
+        <v>632000.0</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="10" t="s">
         <v>79</v>
       </c>
       <c r="H16" s="6"/>
@@ -2248,22 +2266,22 @@
         <v>70</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D17" s="4">
-        <v>284000.0</v>
+        <v>648000.0</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="10" t="s">
         <v>83</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -2289,22 +2307,22 @@
         <v>70</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D18" s="4">
-        <v>350000.0</v>
+        <v>284000.0</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F18" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="F18" s="5" t="s">
         <v>88</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -2330,22 +2348,22 @@
         <v>70</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" s="4">
-        <v>632000.0</v>
+        <v>90</v>
+      </c>
+      <c r="D19" s="11">
+        <v>693000.0</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>92</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>93</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -2371,21 +2389,21 @@
         <v>70</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>94</v>
       </c>
       <c r="D20" s="4">
-        <v>974000.0</v>
+        <v>77000.0</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="5" t="s">
         <v>97</v>
       </c>
       <c r="H20" s="6"/>
@@ -2412,21 +2430,21 @@
         <v>70</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="4">
-        <v>125000.0</v>
+      <c r="D21" s="11">
+        <v>182000.0</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="10" t="s">
         <v>101</v>
       </c>
       <c r="H21" s="6"/>
@@ -2459,15 +2477,15 @@
         <v>103</v>
       </c>
       <c r="D22" s="4">
-        <v>648000.0</v>
+        <v>125000.0</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="10" t="s">
         <v>106</v>
       </c>
       <c r="H22" s="6"/>
@@ -2494,21 +2512,21 @@
         <v>70</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>107</v>
       </c>
       <c r="D23" s="4">
-        <v>77000.0</v>
+        <v>974000.0</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="10" t="s">
         <v>110</v>
       </c>
       <c r="H23" s="6"/>
@@ -2579,19 +2597,19 @@
         <v>112</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="4">
+        <v>2873000.0</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D25" s="4">
-        <v>204234.0</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -2617,22 +2635,22 @@
         <v>111</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="4">
+        <v>204234.0</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="F26" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D26" s="4">
-        <v>331577.0</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="G26" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>125</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -2658,22 +2676,22 @@
         <v>111</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D27" s="4">
         <v>504718.0</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>130</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
@@ -2699,22 +2717,22 @@
         <v>111</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" s="4">
+        <v>331577.0</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D28" s="4">
-        <v>3223000.0</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="F28" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -2740,22 +2758,22 @@
         <v>111</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1620000.0</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D29" s="12">
-        <v>1620000.0</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="F29" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
@@ -2781,22 +2799,22 @@
         <v>111</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" s="4">
+        <v>3223000.0</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D30" s="12">
-        <v>688711.0</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="F30" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>142</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
@@ -2822,13 +2840,13 @@
         <v>111</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="D31" s="4">
-        <v>2873000.0</v>
+        <v>688711.0</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>143</v>
@@ -2869,15 +2887,15 @@
         <v>148</v>
       </c>
       <c r="D32" s="4">
-        <v>872000.0</v>
+        <v>176545.0</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="5" t="s">
         <v>151</v>
       </c>
       <c r="H32" s="6"/>
@@ -2910,15 +2928,15 @@
         <v>152</v>
       </c>
       <c r="D33" s="4">
-        <v>125000.0</v>
+        <v>100244.0</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F33" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G33" s="5" t="s">
         <v>155</v>
       </c>
       <c r="H33" s="6"/>
@@ -2945,22 +2963,22 @@
         <v>146</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D34" s="4">
-        <v>358000.0</v>
+        <v>467099.0</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F34" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="F34" s="5" t="s">
         <v>159</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>160</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2986,22 +3004,22 @@
         <v>146</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D35" s="4">
-        <v>177000.0</v>
+        <v>124000.0</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F35" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="F35" s="5" t="s">
         <v>163</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>164</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -3027,22 +3045,22 @@
         <v>146</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D36" s="4">
-        <v>651000.0</v>
+        <v>335145.0</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F36" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="F36" s="5" t="s">
         <v>167</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -3068,21 +3086,21 @@
         <v>146</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>169</v>
       </c>
       <c r="D37" s="4">
-        <v>3670000.0</v>
-      </c>
-      <c r="E37" s="13" t="s">
+        <v>8982000.0</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="G37" s="11" t="s">
+      <c r="G37" s="5" t="s">
         <v>172</v>
       </c>
       <c r="H37" s="6"/>
@@ -3109,21 +3127,21 @@
         <v>146</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>169</v>
       </c>
       <c r="D38" s="4">
-        <v>3670000.0</v>
+        <v>8982000.0</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="G38" s="5" t="s">
         <v>175</v>
       </c>
       <c r="H38" s="6"/>
@@ -3150,21 +3168,21 @@
         <v>146</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C39" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>176</v>
       </c>
       <c r="D39" s="4">
-        <v>140000.0</v>
+        <v>153000.0</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F39" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="G39" s="5" t="s">
         <v>179</v>
       </c>
       <c r="H39" s="6"/>
@@ -3191,22 +3209,22 @@
         <v>146</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D40" s="4">
-        <v>83000.0</v>
+        <v>796273.0</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="F40" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="G40" s="11" t="s">
+      <c r="F40" s="5" t="s">
         <v>183</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
@@ -3232,22 +3250,22 @@
         <v>146</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D41" s="4">
-        <v>160000.0</v>
+        <v>861365.0</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="F41" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="G41" s="11" t="s">
+      <c r="F41" s="5" t="s">
         <v>187</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>188</v>
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
@@ -3273,21 +3291,21 @@
         <v>146</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D42" s="4">
-        <v>241000.0</v>
+        <v>861365.0</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="F42" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="G42" s="11" t="s">
+      <c r="G42" s="5" t="s">
         <v>191</v>
       </c>
       <c r="H42" s="6"/>
@@ -3314,21 +3332,21 @@
         <v>146</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D43" s="4">
-        <v>667000.0</v>
+        <v>2161000.0</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="F43" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="G43" s="11" t="s">
+      <c r="G43" s="5" t="s">
         <v>195</v>
       </c>
       <c r="H43" s="6"/>
@@ -3355,22 +3373,22 @@
         <v>146</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="C44" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D44" s="4">
+        <v>2161000.0</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D44" s="4">
-        <v>330000.0</v>
-      </c>
-      <c r="E44" s="3" t="s">
+      <c r="F44" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="F44" s="11" t="s">
+      <c r="G44" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="G44" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
@@ -3396,22 +3414,22 @@
         <v>146</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D45" s="4">
-        <v>330000.0</v>
+        <v>2161000.0</v>
       </c>
       <c r="E45" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="G45" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>202</v>
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
@@ -3437,22 +3455,22 @@
         <v>146</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="C46" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D46" s="4">
+        <v>2161000.0</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="D46" s="4">
-        <v>366000.0</v>
-      </c>
-      <c r="E46" s="3" t="s">
+      <c r="G46" s="5" t="s">
         <v>204</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>206</v>
       </c>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
@@ -3478,22 +3496,22 @@
         <v>146</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D47" s="4">
+        <v>2161000.0</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="D47" s="4">
-        <v>1400000.0</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="F47" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="G47" s="11" t="s">
-        <v>211</v>
       </c>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
@@ -3519,22 +3537,22 @@
         <v>146</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D48" s="4">
+        <v>3670000.0</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="G48" s="10" t="s">
         <v>212</v>
-      </c>
-      <c r="D48" s="4">
-        <v>552000.0</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>215</v>
       </c>
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
@@ -3560,22 +3578,22 @@
         <v>146</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D49" s="4">
-        <v>552000.0</v>
+        <v>3670000.0</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>218</v>
+        <v>213</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>215</v>
       </c>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
@@ -3601,22 +3619,22 @@
         <v>146</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D50" s="4">
+        <v>366000.0</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="G50" s="10" t="s">
         <v>219</v>
-      </c>
-      <c r="D50" s="4">
-        <v>427000.0</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>222</v>
       </c>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
@@ -3642,22 +3660,22 @@
         <v>146</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>168</v>
+        <v>208</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D51" s="4">
+        <v>330000.0</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="G51" s="10" t="s">
         <v>223</v>
-      </c>
-      <c r="D51" s="4">
-        <v>1086000.0</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>226</v>
       </c>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
@@ -3683,22 +3701,22 @@
         <v>146</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D52" s="4">
-        <v>861365.0</v>
+        <v>330000.0</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>231</v>
+        <v>224</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>226</v>
       </c>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
@@ -3724,22 +3742,22 @@
         <v>146</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>147</v>
+        <v>208</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>148</v>
+        <v>227</v>
       </c>
       <c r="D53" s="4">
-        <v>872000.0</v>
+        <v>1086000.0</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
@@ -3765,22 +3783,22 @@
         <v>146</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D54" s="4">
-        <v>2161000.0</v>
+        <v>667000.0</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>238</v>
+        <v>232</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>234</v>
       </c>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
@@ -3806,22 +3824,22 @@
         <v>146</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="D55" s="4">
-        <v>861365.0</v>
+        <v>241000.0</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>241</v>
+        <v>236</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>238</v>
       </c>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
@@ -3847,22 +3865,22 @@
         <v>146</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="D56" s="4">
+        <v>140000.0</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="G56" s="10" t="s">
         <v>242</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="D56" s="4">
-        <v>8982000.0</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="G56" s="5" t="s">
-        <v>246</v>
       </c>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
@@ -3888,22 +3906,22 @@
         <v>146</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>242</v>
+        <v>208</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D57" s="4">
-        <v>124000.0</v>
+        <v>160000.0</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>250</v>
+        <v>244</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>246</v>
       </c>
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
@@ -3929,22 +3947,22 @@
         <v>146</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>242</v>
+        <v>208</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D58" s="4">
-        <v>153000.0</v>
+        <v>587857.0</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
@@ -3970,22 +3988,22 @@
         <v>146</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>242</v>
+        <v>208</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="D59" s="4">
-        <v>8982000.0</v>
+        <v>83000.0</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>254</v>
       </c>
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
@@ -4007,26 +4025,26 @@
       <c r="Y59" s="6"/>
     </row>
     <row r="60">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="D60" s="15">
+        <v>122853.0</v>
+      </c>
+      <c r="E60" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="F60" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="G60" s="5" t="s">
         <v>259</v>
-      </c>
-      <c r="D60" s="4">
-        <v>518000.0</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>262</v>
       </c>
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
@@ -4052,22 +4070,22 @@
         <v>146</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D61" s="4">
         <v>545000.0</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
@@ -4093,22 +4111,22 @@
         <v>146</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D62" s="4">
+        <v>872000.0</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="F62" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="G62" s="10" t="s">
         <v>269</v>
-      </c>
-      <c r="D62" s="4">
-        <v>100244.0</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>272</v>
       </c>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
@@ -4134,22 +4152,22 @@
         <v>146</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>168</v>
+        <v>265</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D63" s="4">
-        <v>587857.0</v>
+        <v>872000.0</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
@@ -4175,22 +4193,22 @@
         <v>146</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D64" s="4">
-        <v>176545.0</v>
+        <v>125000.0</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>280</v>
+        <v>274</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>276</v>
       </c>
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
@@ -4216,22 +4234,22 @@
         <v>146</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>227</v>
+        <v>265</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D65" s="4">
-        <v>796273.0</v>
+        <v>177000.0</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="G65" s="5" t="s">
-        <v>284</v>
+        <v>278</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
@@ -4257,22 +4275,22 @@
         <v>146</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>227</v>
+        <v>265</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>235</v>
+        <v>281</v>
       </c>
       <c r="D66" s="4">
-        <v>2161000.0</v>
+        <v>651000.0</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>284</v>
       </c>
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
@@ -4298,22 +4316,22 @@
         <v>146</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>227</v>
+        <v>265</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>235</v>
+        <v>285</v>
       </c>
       <c r="D67" s="4">
-        <v>2161000.0</v>
+        <v>358000.0</v>
       </c>
       <c r="E67" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="G67" s="10" t="s">
         <v>288</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>290</v>
       </c>
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
@@ -4339,13 +4357,13 @@
         <v>146</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>227</v>
+        <v>289</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>235</v>
+        <v>290</v>
       </c>
       <c r="D68" s="4">
-        <v>2161000.0</v>
+        <v>518000.0</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>291</v>
@@ -4353,7 +4371,7 @@
       <c r="F68" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="G68" s="5" t="s">
+      <c r="G68" s="10" t="s">
         <v>293</v>
       </c>
       <c r="H68" s="6"/>
@@ -4380,22 +4398,22 @@
         <v>146</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>227</v>
+        <v>294</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>235</v>
+        <v>295</v>
       </c>
       <c r="D69" s="4">
-        <v>2161000.0</v>
+        <v>552000.0</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="G69" s="5" t="s">
         <v>296</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="G69" s="10" t="s">
+        <v>298</v>
       </c>
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
@@ -4421,22 +4439,22 @@
         <v>146</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>242</v>
+        <v>294</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="D70" s="12">
-        <v>335145.0</v>
+        <v>295</v>
+      </c>
+      <c r="D70" s="4">
+        <v>552000.0</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="F70" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="G70" s="5" t="s">
+      <c r="F70" s="10" t="s">
         <v>300</v>
+      </c>
+      <c r="G70" s="10" t="s">
+        <v>301</v>
       </c>
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
@@ -4462,22 +4480,22 @@
         <v>146</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>242</v>
+        <v>294</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="D71" s="12">
-        <v>467099.0</v>
+        <v>302</v>
+      </c>
+      <c r="D71" s="4">
+        <v>427000.0</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="F71" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="G71" s="5" t="s">
+      <c r="F71" s="10" t="s">
         <v>304</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>305</v>
       </c>
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
@@ -4503,21 +4521,21 @@
         <v>146</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="D72" s="12">
-        <v>246217.0</v>
+      <c r="D72" s="4">
+        <v>1400000.0</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="F72" s="5" t="s">
+      <c r="F72" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="G72" s="5" t="s">
+      <c r="G72" s="10" t="s">
         <v>309</v>
       </c>
       <c r="H72" s="6"/>
@@ -4541,25 +4559,25 @@
     </row>
     <row r="73">
       <c r="A73" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="C73" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="D73" s="4">
+        <v>246217.0</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="D73" s="4">
-        <v>1780000.0</v>
-      </c>
-      <c r="E73" s="3" t="s">
+      <c r="F73" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="F73" s="5" t="s">
+      <c r="G73" s="5" t="s">
         <v>314</v>
-      </c>
-      <c r="G73" s="5" t="s">
-        <v>315</v>
       </c>
       <c r="H73" s="6"/>
       <c r="I73" s="6"/>
@@ -4582,25 +4600,25 @@
     </row>
     <row r="74">
       <c r="A74" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>243</v>
+        <v>317</v>
       </c>
       <c r="D74" s="4">
-        <v>404699.0</v>
+        <v>92730.0</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="H74" s="6"/>
       <c r="I74" s="6"/>
@@ -4623,25 +4641,25 @@
     </row>
     <row r="75">
       <c r="A75" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>319</v>
+        <v>169</v>
       </c>
       <c r="D75" s="4">
-        <v>675218.0</v>
+        <v>404699.0</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="H75" s="6"/>
       <c r="I75" s="6"/>
@@ -4664,25 +4682,25 @@
     </row>
     <row r="76">
       <c r="A76" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D76" s="4">
-        <v>2930000.0</v>
+        <v>1780000.0</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
@@ -4705,25 +4723,25 @@
     </row>
     <row r="77">
       <c r="A77" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="D77" s="4">
-        <v>2930000.0</v>
+        <v>542298.0</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="H77" s="6"/>
       <c r="I77" s="6"/>
@@ -4746,25 +4764,25 @@
     </row>
     <row r="78">
       <c r="A78" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D78" s="4">
-        <v>724305.0</v>
+        <v>2930000.0</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="H78" s="6"/>
       <c r="I78" s="6"/>
@@ -4787,16 +4805,16 @@
     </row>
     <row r="79">
       <c r="A79" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D79" s="4">
-        <v>67542.0</v>
+        <v>2930000.0</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>336</v>
@@ -4828,16 +4846,16 @@
     </row>
     <row r="80">
       <c r="A80" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>339</v>
       </c>
       <c r="D80" s="4">
-        <v>49848.0</v>
+        <v>675218.0</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>340</v>
@@ -4869,25 +4887,25 @@
     </row>
     <row r="81">
       <c r="A81" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D81" s="4">
-        <v>64565.0</v>
+        <v>49848.0</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="H81" s="6"/>
       <c r="I81" s="6"/>
@@ -4910,25 +4928,25 @@
     </row>
     <row r="82">
       <c r="A82" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D82" s="4">
-        <v>1410000.0</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>348</v>
+        <v>4932.0</v>
+      </c>
+      <c r="E82" s="12" t="s">
+        <v>349</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="H82" s="6"/>
       <c r="I82" s="6"/>
@@ -4951,25 +4969,25 @@
     </row>
     <row r="83">
       <c r="A83" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>311</v>
+        <v>343</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D83" s="4">
-        <v>92730.0</v>
+        <v>64565.0</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
@@ -4992,25 +5010,25 @@
     </row>
     <row r="84">
       <c r="A84" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D84" s="4">
-        <v>4932.0</v>
-      </c>
-      <c r="E84" s="13" t="s">
-        <v>356</v>
+        <v>67542.0</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>357</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="H84" s="6"/>
       <c r="I84" s="6"/>
@@ -5033,25 +5051,25 @@
     </row>
     <row r="85">
       <c r="A85" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>311</v>
+        <v>343</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D85" s="4">
-        <v>542298.0</v>
+        <v>1410000.0</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H85" s="6"/>
       <c r="I85" s="6"/>
@@ -5074,25 +5092,25 @@
     </row>
     <row r="86">
       <c r="A86" s="3" t="s">
-        <v>363</v>
+        <v>315</v>
       </c>
       <c r="B86" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="D86" s="4">
+        <v>724305.0</v>
+      </c>
+      <c r="E86" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="D86" s="4">
-        <v>5078000.0</v>
-      </c>
-      <c r="E86" s="3" t="s">
+      <c r="F86" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="F86" s="5" t="s">
+      <c r="G86" s="5" t="s">
         <v>367</v>
-      </c>
-      <c r="G86" s="5" t="s">
-        <v>368</v>
       </c>
       <c r="H86" s="6"/>
       <c r="I86" s="6"/>
@@ -5115,25 +5133,25 @@
     </row>
     <row r="87">
       <c r="A87" s="3" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D87" s="4">
-        <v>5312000.0</v>
+        <v>2280000.0</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="F87" s="5" t="s">
         <v>371</v>
       </c>
+      <c r="F87" s="10" t="s">
+        <v>372</v>
+      </c>
       <c r="G87" s="5" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="H87" s="6"/>
       <c r="I87" s="6"/>
@@ -5156,25 +5174,25 @@
     </row>
     <row r="88">
       <c r="A88" s="3" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D88" s="4">
-        <v>2280000.0</v>
+        <v>5078000.0</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="F88" s="11" t="s">
         <v>375</v>
       </c>
+      <c r="F88" s="5" t="s">
+        <v>376</v>
+      </c>
       <c r="G88" s="5" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H88" s="6"/>
       <c r="I88" s="6"/>
@@ -5197,16 +5215,16 @@
     </row>
     <row r="89">
       <c r="A89" s="3" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>378</v>
       </c>
       <c r="D89" s="4">
-        <v>126255.0</v>
+        <v>5312000.0</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>379</v>
@@ -5238,25 +5256,25 @@
     </row>
     <row r="90">
       <c r="A90" s="3" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D90" s="4">
         <v>1657000.0</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="H90" s="6"/>
       <c r="I90" s="6"/>
@@ -5278,26 +5296,26 @@
       <c r="Y90" s="6"/>
     </row>
     <row r="91">
-      <c r="A91" s="15" t="s">
-        <v>363</v>
-      </c>
-      <c r="B91" s="15" t="s">
-        <v>386</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>386</v>
-      </c>
-      <c r="D91" s="12">
-        <v>5703600.0</v>
-      </c>
-      <c r="E91" s="15" t="s">
+      <c r="A91" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="C91" s="3" t="s">
         <v>387</v>
       </c>
+      <c r="D91" s="4">
+        <v>126255.0</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>388</v>
+      </c>
       <c r="F91" s="5" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="H91" s="6"/>
       <c r="I91" s="6"/>
@@ -5319,13 +5337,27 @@
       <c r="Y91" s="6"/>
     </row>
     <row r="92">
-      <c r="A92" s="6"/>
-      <c r="B92" s="6"/>
-      <c r="C92" s="6"/>
-      <c r="D92" s="6"/>
-      <c r="E92" s="6"/>
-      <c r="F92" s="6"/>
-      <c r="G92" s="6"/>
+      <c r="A92" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="D92" s="4">
+        <v>5703600.0</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>394</v>
+      </c>
       <c r="H92" s="6"/>
       <c r="I92" s="6"/>
       <c r="J92" s="6"/>
@@ -29226,7 +29258,7 @@
     <hyperlink r:id="rId144" ref="G73"/>
     <hyperlink r:id="rId145" ref="F74"/>
     <hyperlink r:id="rId146" ref="G74"/>
-    <hyperlink r:id="rId147" location=":~:text=The%20Graduate%20Program%20in%20Neuroscience,degrees%20in%20Neuroscience." ref="F75"/>
+    <hyperlink r:id="rId147" ref="F75"/>
     <hyperlink r:id="rId148" ref="G75"/>
     <hyperlink r:id="rId149" ref="F76"/>
     <hyperlink r:id="rId150" ref="G76"/>
@@ -29236,7 +29268,7 @@
     <hyperlink r:id="rId154" ref="G78"/>
     <hyperlink r:id="rId155" ref="F79"/>
     <hyperlink r:id="rId156" ref="G79"/>
-    <hyperlink r:id="rId157" ref="F80"/>
+    <hyperlink r:id="rId157" location=":~:text=The%20Graduate%20Program%20in%20Neuroscience,degrees%20in%20Neuroscience." ref="F80"/>
     <hyperlink r:id="rId158" ref="G80"/>
     <hyperlink r:id="rId159" ref="F81"/>
     <hyperlink r:id="rId160" ref="G81"/>
@@ -29260,8 +29292,10 @@
     <hyperlink r:id="rId178" ref="G90"/>
     <hyperlink r:id="rId179" ref="F91"/>
     <hyperlink r:id="rId180" ref="G91"/>
+    <hyperlink r:id="rId181" ref="F92"/>
+    <hyperlink r:id="rId182" ref="G92"/>
   </hyperlinks>
-  <drawing r:id="rId181"/>
+  <drawing r:id="rId183"/>
 </worksheet>
 </file>
 
@@ -29280,62 +29314,62 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>193</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>244</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13">
@@ -29345,97 +29379,97 @@
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>248</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>229</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>236</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>239</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>251</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>